<commit_message>
initial code for 5 pwm outputs
</commit_message>
<xml_diff>
--- a/bt_mesh_sig_rgbcw/DOC/pin分配.xlsx
+++ b/bt_mesh_sig_rgbcw/DOC/pin分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,31 +38,119 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>P22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模拟输入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷达中频输入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>光敏电阻输入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TXD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RXD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU串口发</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU串口收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM输出(控制亮度)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM输出(控制冷暖)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM输出(控制R)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM输出(控制G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM输出(控制B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>P01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>P22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>模拟输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>雷达中频输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>光敏电阻输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P20</t>
+    <t>P02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>外设映射</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PWM11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AN2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AN10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -70,31 +158,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>P04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RXD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCU串口发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCU串口收</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PWM输出(控制亮度)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PWM输出(控制冷暖)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -156,7 +220,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -165,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,11 +532,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -479,7 +544,7 @@
     <col min="5" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -492,8 +557,11 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -501,80 +569,149 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>